<commit_message>
Funções para plotar displacement e internal tensions
</commit_message>
<xml_diff>
--- a/entrada2.xlsx
+++ b/entrada2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riywa\Desktop\APS4_mecsol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70031C1-5232-4FBC-9A6A-DB5ACD7576C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB51AA98-0E6D-41EE-9487-80400A64F9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11124" yWindow="3396" windowWidth="12264" windowHeight="9192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,14 +91,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -522,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -617,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1035,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>